<commit_message>
added some totals and fixed some grammar issure in report
</commit_message>
<xml_diff>
--- a/PCB/SCHEMATICS/FINAL SUBMISSION/BOMJLC-submission.xlsx
+++ b/PCB/SCHEMATICS/FINAL SUBMISSION/BOMJLC-submission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3520\Desktop\EEE3088-group-09\PCB\SCHEMATICS\FINAL SUBMISSION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3904FD3-D506-4B0A-9360-D6F8444B1862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75DA15E-99AF-40DA-8D12-0803AC2DCBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E75288A-14D6-4468-B00A-11B3FD826D53}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>D3</t>
   </si>
   <si>
-    <t>D6-D8</t>
-  </si>
-  <si>
     <t>IC1</t>
   </si>
   <si>
@@ -317,16 +314,19 @@
     <t>SOT-363_L2.0-W1.3-P0.65-LS2.1-BL</t>
   </si>
   <si>
-    <t>R1, R4, R5, R7, R14-R17, R24, R26, R28,R32-R34</t>
-  </si>
-  <si>
-    <t>R18-R21,R25,R27,R29</t>
-  </si>
-  <si>
     <t>D1, D4</t>
   </si>
   <si>
     <t>U6</t>
+  </si>
+  <si>
+    <t>R1, R4, R5, R7, R14,R15,R16,R17, R24, R26, R28,R32,R33,R34</t>
+  </si>
+  <si>
+    <t>D6,D7,D8</t>
+  </si>
+  <si>
+    <t>R18,R19,R20,R21,R25,R27,R29</t>
   </si>
 </sst>
 </file>
@@ -700,7 +700,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,394 +713,394 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="4">
         <v>603</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="4">
         <v>402</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="4">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="4">
         <v>603</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="4">
         <v>603</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="4">
         <v>603</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="4">
         <v>1206</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="4">
         <v>805</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C21" s="4">
         <v>402</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="4">
         <v>1206</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="4">
         <v>402</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>